<commit_message>
Add deployment and component diagram
</commit_message>
<xml_diff>
--- a/StudijaIzvedivosti.xlsx
+++ b/StudijaIzvedivosti.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>Nadogradnja</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Profit:</t>
+  </si>
+  <si>
+    <t>12 (mjeseci)</t>
   </si>
 </sst>
 </file>
@@ -843,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -985,45 +988,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1045,6 +1009,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,7 +1356,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1363,10 +1369,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="22" t="s">
         <v>38</v>
       </c>
@@ -1396,7 +1402,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -1431,7 +1437,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="26" t="s">
         <v>2</v>
       </c>
@@ -1464,7 +1470,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="59"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="26" t="s">
         <v>3</v>
       </c>
@@ -1497,7 +1503,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="60"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="27" t="s">
         <v>4</v>
       </c>
@@ -1530,10 +1536,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="62"/>
+      <c r="B6" s="69"/>
       <c r="C6" s="16">
         <f>AVERAGE(C2:C5)</f>
         <v>2.25</v>
@@ -1572,7 +1578,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="72" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
@@ -1607,7 +1613,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="59"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="26" t="s">
         <v>2</v>
       </c>
@@ -1640,7 +1646,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="59"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="26" t="s">
         <v>3</v>
       </c>
@@ -1673,7 +1679,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="60"/>
+      <c r="A10" s="67"/>
       <c r="B10" s="27" t="s">
         <v>4</v>
       </c>
@@ -1696,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" s="9">
         <v>2</v>
@@ -1706,10 +1712,10 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="62"/>
+      <c r="B11" s="69"/>
       <c r="C11" s="16">
         <f>AVERAGE(C7:C10)</f>
         <v>3.25</v>
@@ -1736,7 +1742,7 @@
       </c>
       <c r="I11" s="16">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
       <c r="J11" s="16">
         <f t="shared" si="1"/>
@@ -1748,7 +1754,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="72" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="25" t="s">
@@ -1773,7 +1779,7 @@
         <v>3</v>
       </c>
       <c r="I12" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J12" s="12">
         <v>3</v>
@@ -1783,7 +1789,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="59"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="26" t="s">
         <v>2</v>
       </c>
@@ -1816,7 +1822,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="59"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="26" t="s">
         <v>3</v>
       </c>
@@ -1839,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J14" s="7">
         <v>2</v>
@@ -1849,7 +1855,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="60"/>
+      <c r="A15" s="67"/>
       <c r="B15" s="27" t="s">
         <v>4</v>
       </c>
@@ -1882,10 +1888,10 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="64"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="16">
         <f>AVERAGE(C12:C15)</f>
         <v>1.25</v>
@@ -1912,7 +1918,7 @@
       </c>
       <c r="I16" s="16">
         <f t="shared" si="2"/>
-        <v>2.25</v>
+        <v>1.5</v>
       </c>
       <c r="J16" s="16">
         <f t="shared" si="2"/>
@@ -1937,7 +1943,7 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="58" t="s">
+      <c r="A18" s="65" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="25" t="s">
@@ -1958,7 +1964,7 @@
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="59"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="26" t="s">
         <v>5</v>
       </c>
@@ -1976,12 +1982,14 @@
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="I19" s="76" t="s">
+        <v>12</v>
+      </c>
       <c r="J19" s="7"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="60"/>
+      <c r="A20" s="67"/>
       <c r="B20" s="27" t="s">
         <v>7</v>
       </c>
@@ -1991,9 +1999,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
-      <c r="I20" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="I20" s="20"/>
       <c r="J20" s="20" t="s">
         <v>12</v>
       </c>
@@ -2022,7 +2028,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2030,7 +2036,7 @@
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.21875" customWidth="1"/>
     <col min="7" max="7" width="22.5546875" customWidth="1"/>
     <col min="8" max="8" width="25.5546875" customWidth="1"/>
@@ -2040,7 +2046,7 @@
       <c r="A1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="58" t="s">
         <v>48</v>
       </c>
       <c r="C1" s="30"/>
@@ -2059,7 +2065,7 @@
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
-      <c r="G3" s="70" t="s">
+      <c r="G3" s="57" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2076,10 +2082,10 @@
       <c r="D4" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="60" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2097,11 +2103,11 @@
         <f>B5*C5</f>
         <v>600</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="61">
         <v>1000</v>
       </c>
-      <c r="H5" s="74">
-        <v>40</v>
+      <c r="H5" s="61">
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2118,12 +2124,12 @@
         <f t="shared" ref="D6:D9" si="0">B6*C6</f>
         <v>2100</v>
       </c>
-      <c r="G6" s="75" t="s">
+      <c r="G6" s="62" t="s">
         <v>45</v>
       </c>
       <c r="H6">
         <f>G5*H5</f>
-        <v>40000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2155,7 +2161,7 @@
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="E8" s="69" t="s">
+      <c r="E8" s="56" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2177,12 +2183,12 @@
         <f>SUM(D5:D9)</f>
         <v>5250</v>
       </c>
-      <c r="G9" s="75" t="s">
+      <c r="G9" s="62" t="s">
         <v>50</v>
       </c>
       <c r="H9">
         <f>H6-D24</f>
-        <v>13010</v>
+        <v>8010</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2227,7 +2233,7 @@
         <f>B13*C13</f>
         <v>2500</v>
       </c>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="56" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2317,14 +2323,14 @@
       <c r="A21" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="41">
-        <v>12</v>
+      <c r="B21" s="41" t="s">
+        <v>51</v>
       </c>
       <c r="C21" s="42">
         <v>1220</v>
       </c>
       <c r="D21" s="54">
-        <f t="shared" ref="D21:D22" si="1">B21*C21</f>
+        <f>12*C21</f>
         <v>14640</v>
       </c>
     </row>
@@ -2339,10 +2345,10 @@
         <v>600</v>
       </c>
       <c r="D22" s="51">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D21:D22" si="1">B22*C22</f>
         <v>600</v>
       </c>
-      <c r="E22" s="69" t="s">
+      <c r="E22" s="56" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2357,11 +2363,11 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="73" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="75"/>
       <c r="D24" s="55">
         <f>SUM(D1:D23)</f>
         <v>26990</v>
@@ -2377,15 +2383,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101007AFC1106DB8A04488E866355A5CEB218" ma:contentTypeVersion="2" ma:contentTypeDescription="Stvaranje novog dokumenta." ma:contentTypeScope="" ma:versionID="cf5653b097a0dc1db313e4d0258d9f51">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d34a4129-52ec-4ee5-bc77-23d8e5f94cfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c81d14dc3ad95f274f0f0999b8e60d5" ns2:_="">
     <xsd:import namespace="d34a4129-52ec-4ee5-bc77-23d8e5f94cfd"/>
@@ -2445,6 +2442,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
@@ -2454,14 +2460,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5758EF3-F7D3-4420-8E13-AF1AC80FD17D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{033D9B50-45AF-432E-87DC-2944701B1988}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2474,6 +2472,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5758EF3-F7D3-4420-8E13-AF1AC80FD17D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>